<commit_message>
Deploying to gh-pages from  @ 4590d95235ff7e3d2b8b8f7bf5fa3ade9830fa84 🚀
</commit_message>
<xml_diff>
--- a/assets/excel/2022_1-2-7.xlsx
+++ b/assets/excel/2022_1-2-7.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Hannover\Dez15-Uebergreifende-Analysen\Projekte\Integrationsmonitoring\github\MT_Site\assets\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A469CA6-4BE3-43CF-82CE-54A04FD061F0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3618C50A-319B-44AD-9B98-90F44B6712A9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14010" xr2:uid="{FC67E612-DC3D-4763-BC26-652EFCA3DFEB}"/>
   </bookViews>
@@ -556,7 +556,7 @@
     <t>insgesamt</t>
   </si>
   <si>
-    <t>© Landesamt für Statistik Niedersachsen, Hannover 2021,                                                                          </t>
+    <t>© Landesamt für Statistik Niedersachsen, Hannover 2022,                                                                          </t>
   </si>
   <si>
     <t>Braunschweig, Stadt</t>
@@ -1369,13 +1369,11 @@
   <sheetPr codeName="Tabelle1"/>
   <dimension ref="B1:L1065"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A902" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="D911" sqref="D911"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" customWidth="1"/>
+    <col min="1" max="1" width="5.7109375" customWidth="1"/>
     <col min="2" max="3" width="10.7109375" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="18.85546875" customWidth="1"/>
   </cols>

</xml_diff>